<commit_message>
handle date of change when import employee
</commit_message>
<xml_diff>
--- a/src/Assets/user.xlsx
+++ b/src/Assets/user.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="138">
   <si>
     <t xml:space="preserve">nik (sebagai acuan)</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t xml:space="preserve">tanggal_lensa_berikutnya</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tanggal_ubah_status</t>
   </si>
   <si>
     <t xml:space="preserve">01234</t>
@@ -641,10 +644,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:U2"/>
+  <dimension ref="A1:V2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G10" activeCellId="0" sqref="G10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="P1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="U6" activeCellId="0" sqref="U6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -732,19 +735,22 @@
       <c r="U1" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="V1" s="0" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E2" s="2" t="n">
         <v>43882</v>
@@ -753,34 +759,34 @@
         <v>5</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="O2" s="0" t="n">
         <v>12</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Q2" s="2" t="n">
         <v>42139</v>
@@ -796,6 +802,9 @@
       </c>
       <c r="U2" s="4" t="n">
         <v>44185</v>
+      </c>
+      <c r="V2" s="2" t="n">
+        <v>42231</v>
       </c>
     </row>
   </sheetData>
@@ -843,477 +852,477 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="6" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="6" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="6" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="6" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="6" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="6" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="6" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="6" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="6" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="6" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="6" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="6" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="6" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="6" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="8" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="8" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="8" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="8" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="8" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="8" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="8" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="8" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="8" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="8" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="8" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="8" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="8" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="8" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="8" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="8" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="8" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="8" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="8" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="8" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="8" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="8" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="8" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="8" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="8" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="8" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="8" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="8" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="8" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="8" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="8" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="8" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="8" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="8" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="8" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="8" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="8" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="8" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="8" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="8" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="8" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="8" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="8" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>

</xml_diff>